<commit_message>
editing district data and shapes
</commit_message>
<xml_diff>
--- a/data/old_results/2013_presidential/2013Bulawayol_Presidential_Results_Formatted_13-08-2013.xlsx
+++ b/data/old_results/2013_presidential/2013Bulawayol_Presidential_Results_Formatted_13-08-2013.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\office\Desktop\DI\Zimbabwe_election\data\old_results\2013_presidential\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4E38F334-9035-4B38-A5E6-037D3CA30590}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B406E2D2-6CB4-4EA8-9A49-90358D1BAF26}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="436">
   <si>
     <t>Local Authority</t>
   </si>
@@ -1357,6 +1357,15 @@
   </si>
   <si>
     <t>Bulawayo</t>
+  </si>
+  <si>
+    <t>districtShape 89</t>
+  </si>
+  <si>
+    <t>district shape 60</t>
+  </si>
+  <si>
+    <t>Sum this together for the bulawyo district</t>
   </si>
 </sst>
 </file>
@@ -1372,12 +1381,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1392,11 +1407,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8508,55 +8526,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3260524B-C99F-4B77-BC2F-0EFC7FE230FA}">
-  <dimension ref="A3:B7"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>430</v>
       </c>
       <c r="B3" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>431</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D4:D6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>